<commit_message>
added enbridge 2022 nos dates
</commit_message>
<xml_diff>
--- a/Analysis/net_energy_dates.xlsx
+++ b/Analysis/net_energy_dates.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mossgran\Documents\ne2\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32414809-7284-454B-9D05-7FF008852149}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2835" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="holidays" sheetId="1" r:id="rId1"/>
@@ -249,7 +250,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -279,10 +280,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,20 +562,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -586,7 +586,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -597,7 +597,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -608,7 +608,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -619,7 +619,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -630,7 +630,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -641,7 +641,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2020</v>
       </c>
@@ -652,7 +652,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2020</v>
       </c>
@@ -663,7 +663,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -674,7 +674,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2020</v>
       </c>
@@ -685,7 +685,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2020</v>
       </c>
@@ -696,7 +696,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -707,7 +707,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2020</v>
       </c>
@@ -718,7 +718,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2020</v>
       </c>
@@ -729,7 +729,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2020</v>
       </c>
@@ -740,7 +740,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2019</v>
       </c>
@@ -751,7 +751,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -762,7 +762,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2019</v>
       </c>
@@ -773,7 +773,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2019</v>
       </c>
@@ -784,7 +784,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2019</v>
       </c>
@@ -795,7 +795,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2019</v>
       </c>
@@ -806,7 +806,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2019</v>
       </c>
@@ -817,7 +817,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -828,7 +828,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2019</v>
       </c>
@@ -839,7 +839,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2019</v>
       </c>
@@ -850,7 +850,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -861,7 +861,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2019</v>
       </c>
@@ -872,7 +872,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2019</v>
       </c>
@@ -883,7 +883,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2019</v>
       </c>
@@ -894,7 +894,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2018</v>
       </c>
@@ -905,7 +905,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>2018</v>
       </c>
@@ -916,7 +916,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2018</v>
       </c>
@@ -927,7 +927,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2018</v>
       </c>
@@ -938,7 +938,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2018</v>
       </c>
@@ -949,7 +949,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2018</v>
       </c>
@@ -960,7 +960,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2018</v>
       </c>
@@ -971,7 +971,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2018</v>
       </c>
@@ -982,7 +982,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2018</v>
       </c>
@@ -993,7 +993,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2018</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2018</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2018</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2018</v>
       </c>
@@ -1044,20 +1044,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1074,887 +1076,1091 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B2" s="1">
-        <v>44197</v>
+        <v>44593</v>
       </c>
       <c r="C2" s="1">
-        <v>44166</v>
+        <v>44565</v>
       </c>
       <c r="D2" s="1">
-        <v>44179</v>
+        <v>44578</v>
       </c>
       <c r="E2" s="1">
-        <v>44180</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44579</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B3" s="1">
-        <v>44228</v>
+        <v>44621</v>
       </c>
       <c r="C3" s="1">
-        <v>44200</v>
+        <v>44593</v>
       </c>
       <c r="D3" s="1">
-        <v>44211</v>
+        <v>44603</v>
       </c>
       <c r="E3" s="1">
-        <v>44214</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44606</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B4" s="1">
-        <v>44256</v>
+        <v>44652</v>
       </c>
       <c r="C4" s="1">
-        <v>44228</v>
+        <v>44621</v>
       </c>
       <c r="D4" s="1">
-        <v>44238</v>
+        <v>44637</v>
       </c>
       <c r="E4" s="1">
-        <v>44239</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44638</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B5" s="1">
-        <v>44287</v>
+        <v>44682</v>
       </c>
       <c r="C5" s="1">
-        <v>44256</v>
+        <v>44652</v>
       </c>
       <c r="D5" s="1">
-        <v>44270</v>
+        <v>44665</v>
       </c>
       <c r="E5" s="1">
-        <v>44271</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B6" s="1">
-        <v>44317</v>
+        <v>44713</v>
       </c>
       <c r="C6" s="1">
-        <v>44287</v>
+        <v>44683</v>
       </c>
       <c r="D6" s="1">
-        <v>44302</v>
+        <v>44697</v>
       </c>
       <c r="E6" s="1">
-        <v>44305</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44698</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B7" s="1">
-        <v>44348</v>
+        <v>44743</v>
       </c>
       <c r="C7" s="1">
-        <v>44319</v>
+        <v>44713</v>
       </c>
       <c r="D7" s="1">
-        <v>44330</v>
+        <v>44727</v>
       </c>
       <c r="E7" s="1">
-        <v>44333</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44728</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B8" s="1">
-        <v>44378</v>
+        <v>44774</v>
       </c>
       <c r="C8" s="1">
-        <v>44348</v>
+        <v>44746</v>
       </c>
       <c r="D8" s="1">
-        <v>44361</v>
+        <v>44757</v>
       </c>
       <c r="E8" s="1">
-        <v>44362</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44760</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B9" s="1">
-        <v>44409</v>
+        <v>44805</v>
       </c>
       <c r="C9" s="1">
-        <v>44379</v>
+        <v>44775</v>
       </c>
       <c r="D9" s="1">
-        <v>44393</v>
+        <v>44790</v>
       </c>
       <c r="E9" s="1">
-        <v>44396</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44791</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B10" s="1">
-        <v>44440</v>
+        <v>44835</v>
       </c>
       <c r="C10" s="1">
-        <v>44411</v>
+        <v>44805</v>
       </c>
       <c r="D10" s="1">
-        <v>44425</v>
+        <v>44819</v>
       </c>
       <c r="E10" s="1">
-        <v>44426</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44820</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B11" s="1">
-        <v>44470</v>
+        <v>44866</v>
       </c>
       <c r="C11" s="1">
-        <v>44440</v>
+        <v>44837</v>
       </c>
       <c r="D11" s="1">
-        <v>44455</v>
+        <v>44851</v>
       </c>
       <c r="E11" s="1">
-        <v>44456</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44852</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B12" s="1">
-        <v>44501</v>
+        <v>44896</v>
       </c>
       <c r="C12" s="1">
-        <v>44470</v>
+        <v>44866</v>
       </c>
       <c r="D12" s="1">
-        <v>44484</v>
+        <v>44881</v>
       </c>
       <c r="E12" s="1">
-        <v>44487</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44882</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="B13" s="1">
-        <v>44531</v>
+        <v>44927</v>
       </c>
       <c r="C13" s="1">
-        <v>44501</v>
+        <v>44896</v>
       </c>
       <c r="D13" s="1">
-        <v>44515</v>
+        <v>44908</v>
       </c>
       <c r="E13" s="1">
-        <v>44516</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44909</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2021</v>
       </c>
       <c r="B14" s="1">
+        <v>44197</v>
+      </c>
+      <c r="C14" s="1">
+        <v>44166</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44179</v>
+      </c>
+      <c r="E14" s="1">
+        <v>44180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2021</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44228</v>
+      </c>
+      <c r="C15" s="1">
+        <v>44200</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44211</v>
+      </c>
+      <c r="E15" s="1">
+        <v>44214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2021</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44256</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44228</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44238</v>
+      </c>
+      <c r="E16" s="1">
+        <v>44239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>2021</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44287</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44256</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44270</v>
+      </c>
+      <c r="E17" s="1">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>2021</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44317</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44287</v>
+      </c>
+      <c r="D18" s="1">
+        <v>44302</v>
+      </c>
+      <c r="E18" s="1">
+        <v>44305</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2021</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44348</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44319</v>
+      </c>
+      <c r="D19" s="1">
+        <v>44330</v>
+      </c>
+      <c r="E19" s="1">
+        <v>44333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>2021</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44378</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44348</v>
+      </c>
+      <c r="D20" s="1">
+        <v>44361</v>
+      </c>
+      <c r="E20" s="1">
+        <v>44362</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2021</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44409</v>
+      </c>
+      <c r="C21" s="1">
+        <v>44379</v>
+      </c>
+      <c r="D21" s="1">
+        <v>44393</v>
+      </c>
+      <c r="E21" s="1">
+        <v>44396</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2021</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44440</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44411</v>
+      </c>
+      <c r="D22" s="1">
+        <v>44425</v>
+      </c>
+      <c r="E22" s="1">
+        <v>44426</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2021</v>
+      </c>
+      <c r="B23" s="1">
+        <v>44470</v>
+      </c>
+      <c r="C23" s="1">
+        <v>44440</v>
+      </c>
+      <c r="D23" s="1">
+        <v>44455</v>
+      </c>
+      <c r="E23" s="1">
+        <v>44456</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2021</v>
+      </c>
+      <c r="B24" s="1">
+        <v>44501</v>
+      </c>
+      <c r="C24" s="1">
+        <v>44470</v>
+      </c>
+      <c r="D24" s="1">
+        <v>44484</v>
+      </c>
+      <c r="E24" s="1">
+        <v>44487</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2021</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44531</v>
+      </c>
+      <c r="C25" s="1">
+        <v>44501</v>
+      </c>
+      <c r="D25" s="1">
+        <v>44515</v>
+      </c>
+      <c r="E25" s="1">
+        <v>44516</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2021</v>
+      </c>
+      <c r="B26" s="1">
         <v>44562</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C26" s="1">
         <v>44531</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D26" s="1">
         <v>44544</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E26" s="1">
         <v>44545</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2020</v>
-      </c>
-      <c r="B15" s="1">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2020</v>
+      </c>
+      <c r="B27" s="1">
         <v>43831</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C27" s="1">
         <v>43801</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D27" s="1">
         <v>43812</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E27" s="1">
         <v>43815</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2020</v>
-      </c>
-      <c r="B16" s="1">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2020</v>
+      </c>
+      <c r="B28" s="1">
         <v>43862</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C28" s="1">
         <v>43832</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D28" s="1">
         <v>43846</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E28" s="1">
         <v>43847</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2020</v>
-      </c>
-      <c r="B17" s="1">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2020</v>
+      </c>
+      <c r="B29" s="1">
         <v>43891</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C29" s="1">
         <v>43864</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D29" s="1">
         <v>43874</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E29" s="1">
         <v>43875</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2020</v>
-      </c>
-      <c r="B18" s="1">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2020</v>
+      </c>
+      <c r="B30" s="1">
         <v>43922</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C30" s="1">
         <v>43892</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D30" s="1">
         <v>43906</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E30" s="1">
         <v>43907</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2020</v>
-      </c>
-      <c r="B19" s="1">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>2020</v>
+      </c>
+      <c r="B31" s="1">
         <v>43952</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C31" s="1">
         <v>43922</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D31" s="1">
         <v>43937</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E31" s="1">
         <v>43938</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>2020</v>
-      </c>
-      <c r="B20" s="1">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>2020</v>
+      </c>
+      <c r="B32" s="1">
         <v>43983</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C32" s="1">
         <v>43952</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D32" s="1">
         <v>43965</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E32" s="1">
         <v>43966</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2020</v>
-      </c>
-      <c r="B21" s="1">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2020</v>
+      </c>
+      <c r="B33" s="1">
         <v>44013</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C33" s="1">
         <v>43983</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D33" s="1">
         <v>43997</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E33" s="1">
         <v>43998</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2020</v>
-      </c>
-      <c r="B22" s="1">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>2020</v>
+      </c>
+      <c r="B34" s="1">
         <v>44044</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C34" s="1">
         <v>44014</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D34" s="1">
         <v>44028</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E34" s="1">
         <v>44029</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2020</v>
-      </c>
-      <c r="B23" s="1">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>2020</v>
+      </c>
+      <c r="B35" s="1">
         <v>44075</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C35" s="1">
         <v>44047</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D35" s="1">
         <v>44060</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E35" s="1">
         <v>44061</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2020</v>
-      </c>
-      <c r="B24" s="1">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>2020</v>
+      </c>
+      <c r="B36" s="1">
         <v>44105</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C36" s="1">
         <v>44075</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D36" s="1">
         <v>44090</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E36" s="1">
         <v>44091</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2020</v>
-      </c>
-      <c r="B25" s="1">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>2020</v>
+      </c>
+      <c r="B37" s="1">
         <v>44136</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C37" s="1">
         <v>44105</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D37" s="1">
         <v>44120</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E37" s="1">
         <v>44123</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2020</v>
-      </c>
-      <c r="B26" s="1">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>2020</v>
+      </c>
+      <c r="B38" s="1">
         <v>44166</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C38" s="1">
         <v>44137</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D38" s="1">
         <v>44151</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E38" s="1">
         <v>44152</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2020</v>
-      </c>
-      <c r="B27" s="1">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>2020</v>
+      </c>
+      <c r="B39" s="1">
         <v>44197</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C39" s="1">
         <v>44166</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D39" s="1">
         <v>44179</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E39" s="1">
         <v>44180</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>2019</v>
-      </c>
-      <c r="B28" s="1">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>2019</v>
+      </c>
+      <c r="B40" s="1">
         <v>43466</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C40" s="1">
         <v>43437</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D40" s="1">
         <v>43447</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E40" s="1">
         <v>43448</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>2019</v>
-      </c>
-      <c r="B29" s="1">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>2019</v>
+      </c>
+      <c r="B41" s="1">
         <v>43497</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C41" s="1">
         <v>43467</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D41" s="1">
         <v>43481</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E41" s="1">
         <v>43482</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>2019</v>
-      </c>
-      <c r="B30" s="1">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>2019</v>
+      </c>
+      <c r="B42" s="1">
         <v>43525</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C42" s="1">
         <v>43497</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D42" s="1">
         <v>43509</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E42" s="1">
         <v>43510</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>2019</v>
-      </c>
-      <c r="B31" s="1">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>2019</v>
+      </c>
+      <c r="B43" s="1">
         <v>43556</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C43" s="1">
         <v>43525</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D43" s="1">
         <v>43539</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E43" s="1">
         <v>43542</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>2019</v>
-      </c>
-      <c r="B32" s="1">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>2019</v>
+      </c>
+      <c r="B44" s="1">
         <v>43586</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C44" s="1">
         <v>43556</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D44" s="1">
         <v>43570</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E44" s="1">
         <v>43571</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>2019</v>
-      </c>
-      <c r="B33" s="1">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>2019</v>
+      </c>
+      <c r="B45" s="1">
         <v>43617</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C45" s="1">
         <v>43586</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D45" s="1">
         <v>43601</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E45" s="1">
         <v>43602</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>2019</v>
-      </c>
-      <c r="B34" s="1">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>2019</v>
+      </c>
+      <c r="B46" s="1">
         <v>43647</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C46" s="1">
         <v>43619</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D46" s="1">
         <v>43630</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E46" s="1">
         <v>43633</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>2019</v>
-      </c>
-      <c r="B35" s="1">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>2019</v>
+      </c>
+      <c r="B47" s="1">
         <v>43678</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C47" s="1">
         <v>43648</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D47" s="1">
         <v>43662</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E47" s="1">
         <v>43663</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>2019</v>
-      </c>
-      <c r="B36" s="1">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>2019</v>
+      </c>
+      <c r="B48" s="1">
         <v>43709</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C48" s="1">
         <v>43678</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D48" s="1">
         <v>43692</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E48" s="1">
         <v>43693</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>2019</v>
-      </c>
-      <c r="B37" s="1">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2019</v>
+      </c>
+      <c r="B49" s="1">
         <v>43739</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C49" s="1">
         <v>43711</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D49" s="1">
         <v>43721</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E49" s="1">
         <v>43724</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>2019</v>
-      </c>
-      <c r="B38" s="1">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2019</v>
+      </c>
+      <c r="B50" s="1">
         <v>43770</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C50" s="1">
         <v>43739</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D50" s="1">
         <v>43754</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E50" s="1">
         <v>43755</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>2019</v>
-      </c>
-      <c r="B39" s="1">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>2019</v>
+      </c>
+      <c r="B51" s="1">
         <v>43800</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C51" s="1">
         <v>43770</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D51" s="1">
         <v>43783</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E51" s="1">
         <v>43784</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>2019</v>
-      </c>
-      <c r="B40" s="1">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2019</v>
+      </c>
+      <c r="B52" s="1">
         <v>43831</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C52" s="1">
         <v>43801</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D52" s="1">
         <v>43812</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E52" s="1">
         <v>43815</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>2018</v>
-      </c>
-      <c r="B41" s="1">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>2018</v>
+      </c>
+      <c r="B53" s="1">
         <v>43101</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C53" s="1">
         <v>43070</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D53" s="1">
         <v>43083</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E53" s="1">
         <v>43084</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>2018</v>
-      </c>
-      <c r="B42" s="1">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>2018</v>
+      </c>
+      <c r="B54" s="1">
         <v>43132</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C54" s="1">
         <v>43102</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D54" s="1">
         <v>43116</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E54" s="1">
         <v>43117</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>2018</v>
-      </c>
-      <c r="B43" s="1">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>2018</v>
+      </c>
+      <c r="B55" s="1">
         <v>43160</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C55" s="1">
         <v>43132</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D55" s="1">
         <v>43144</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E55" s="1">
         <v>43145</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>2018</v>
-      </c>
-      <c r="B44" s="1">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>2018</v>
+      </c>
+      <c r="B56" s="1">
         <v>43191</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C56" s="1">
         <v>43160</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D56" s="1">
         <v>43174</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E56" s="1">
         <v>43175</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>2018</v>
-      </c>
-      <c r="B45" s="1">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>2018</v>
+      </c>
+      <c r="B57" s="1">
         <v>43221</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C57" s="1">
         <v>43192</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D57" s="1">
         <v>43203</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E57" s="1">
         <v>43206</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>2018</v>
-      </c>
-      <c r="B46" s="1">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>2018</v>
+      </c>
+      <c r="B58" s="1">
         <v>43252</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C58" s="1">
         <v>43221</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D58" s="1">
         <v>43236</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E58" s="1">
         <v>43237</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>2018</v>
-      </c>
-      <c r="B47" s="1">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>2018</v>
+      </c>
+      <c r="B59" s="1">
         <v>43282</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C59" s="1">
         <v>43252</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D59" s="1">
         <v>43265</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E59" s="1">
         <v>43266</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>2018</v>
-      </c>
-      <c r="B48" s="1">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>2018</v>
+      </c>
+      <c r="B60" s="1">
         <v>43313</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C60" s="1">
         <v>43284</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D60" s="1">
         <v>43297</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E60" s="1">
         <v>43298</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>2018</v>
-      </c>
-      <c r="B49" s="1">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>2018</v>
+      </c>
+      <c r="B61" s="1">
         <v>43344</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C61" s="1">
         <v>43313</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D61" s="1">
         <v>43328</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E61" s="1">
         <v>43329</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>2018</v>
-      </c>
-      <c r="B50" s="1">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>2018</v>
+      </c>
+      <c r="B62" s="1">
         <v>43374</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C62" s="1">
         <v>43347</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D62" s="1">
         <v>43357</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E62" s="1">
         <v>43360</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>2018</v>
-      </c>
-      <c r="B51" s="1">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>2018</v>
+      </c>
+      <c r="B63" s="1">
         <v>43405</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C63" s="1">
         <v>43374</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D63" s="1">
         <v>43389</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E63" s="1">
         <v>43390</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>2018</v>
-      </c>
-      <c r="B52" s="1">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>2018</v>
+      </c>
+      <c r="B64" s="1">
         <v>43435</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C64" s="1">
         <v>43405</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D64" s="1">
         <v>43419</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E64" s="1">
         <v>43420</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>2018</v>
-      </c>
-      <c r="B53" s="1">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>2018</v>
+      </c>
+      <c r="B65" s="1">
         <v>43466</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C65" s="1">
         <v>43437</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D65" s="1">
         <v>43447</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E65" s="1">
         <v>43448</v>
       </c>
     </row>

</xml_diff>